<commit_message>
updating the risk on the sql injection with mitigation
</commit_message>
<xml_diff>
--- a/risks.xlsx
+++ b/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
   <si>
     <t>Severity</t>
   </si>
@@ -208,6 +208,21 @@
     <t>missing-hardening@aws-secret-manager-vault</t>
   </si>
   <si>
+    <t>in Discussion</t>
+  </si>
+  <si>
+    <t>The hardening measures on the docker images are completed, the network ones in progress</t>
+  </si>
+  <si>
+    <t>2023-01-10</t>
+  </si>
+  <si>
+    <t>Ciro Bologna</t>
+  </si>
+  <si>
+    <t>XYZ-1234</t>
+  </si>
+  <si>
     <t>Missing Hardening risk at Backend</t>
   </si>
   <si>
@@ -217,18 +232,276 @@
     <t>Very Likely</t>
   </si>
   <si>
+    <t>CWE-501</t>
+  </si>
+  <si>
+    <t>Unguarded Access From Internet</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Backend by Frontend via User Traffic</t>
+  </si>
+  <si>
+    <t>Encapsulation of Technical Asset</t>
+  </si>
+  <si>
+    <t>Encapsulate the asset behind a guarding service, application, or reverse-proxy. For admin maintenance a bastion-host should be used as a jump-server. For file transfer a store-and-forward-host should be used as an indirect file exchange platform.</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@backend@frontend@frontend&gt;user-traffic</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>CWE-502</t>
+  </si>
+  <si>
+    <t>Untrusted Deserialization</t>
+  </si>
+  <si>
+    <t>Untrusted Deserialization risk at Database</t>
+  </si>
+  <si>
+    <t>Prevention of Deserialization of Untrusted Data</t>
+  </si>
+  <si>
+    <t>Try to avoid the deserialization of untrusted data (even of data within the same trust-boundary as long as it is sent across a remote connection) in order to stay safe from Untrusted Deserialization vulnerabilities. Alternatively a strict whitelisting approach of the classes/types/values to deserialize might help as well. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>untrusted-deserialization@database</t>
+  </si>
+  <si>
+    <t>CWE-912</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Backend</t>
+  </si>
+  <si>
+    <t>Container Infrastructure Hardening</t>
+  </si>
+  <si>
+    <t>Apply hardening of all container infrastructures (see for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; and the &lt;i&gt;Docker Bench for Security&lt;/i&gt;). Use only trusted base images of the original vendors, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;i&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Regularly execute container image scans with tools checking the layers for vulnerable components.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS/CSVS applied?</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@backend</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Database</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@database</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Frontend</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@frontend</t>
+  </si>
+  <si>
+    <t>CWE-1127</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure</t>
+  </si>
+  <si>
+    <t>Missing Build Infrastructure in the threat model (referencing asset Backend as an example)</t>
+  </si>
+  <si>
+    <t>Build Pipeline Hardening</t>
+  </si>
+  <si>
+    <t>Include the build infrastructure in the model.</t>
+  </si>
+  <si>
+    <t>missing-build-infrastructure@backend</t>
+  </si>
+  <si>
+    <t>CWE-308</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication (2FA)</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link User Traffic from Frontend to Backend</t>
+  </si>
+  <si>
+    <t>Authentication with Second Factor (2FA)</t>
+  </si>
+  <si>
+    <t>Apply an authentication method to the technical asset protecting highly sensitive data via two-factor authentication for human users.</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@frontend&gt;user-traffic@frontend@backend</t>
+  </si>
+  <si>
+    <t>Missing Vault Isolation</t>
+  </si>
+  <si>
+    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset AWS Secret Manager Vault against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>Network Segmentation</t>
+  </si>
+  <si>
+    <t>Apply a network segmentation trust-boundary around the highly sensitive vault assets and their datastores.</t>
+  </si>
+  <si>
+    <t>missing-vault-isolation@aws-secret-manager-vault</t>
+  </si>
+  <si>
+    <t>Missing Web Application Firewall (WAF)</t>
+  </si>
+  <si>
+    <t>Missing Web Application Firewall (WAF) risk at Backend</t>
+  </si>
+  <si>
+    <t>Web Application Firewall (WAF)</t>
+  </si>
+  <si>
+    <t>Consider placing a Web Application Firewall (WAF) in front of the web-services and/or web-applications. For cloud environments many cloud providers offer pre-configured WAFs. Even reverse proxies can be enhances by a WAF component via ModSecurity plugins.</t>
+  </si>
+  <si>
+    <t>Is a Web Application Firewall (WAF) in place?</t>
+  </si>
+  <si>
+    <t>missing-waf@backend</t>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+  </si>
+  <si>
     <t>Development</t>
   </si>
   <si>
+    <t>CWE-918</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF)</t>
+  </si>
+  <si>
+    <t>Vault Access (backend)</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at Backend server-side web-requesting the target AWS Secret Manager Vault via Vault Access (backend)</t>
+  </si>
+  <si>
+    <t>SSRF Prevention</t>
+  </si>
+  <si>
+    <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@backend@aws-secret-manager-vault@backend&gt;vault-access-backend</t>
+  </si>
+  <si>
+    <t>CWE-319</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication</t>
+  </si>
+  <si>
+    <t>Server Traffic</t>
+  </si>
+  <si>
+    <t>Unencrypted Communication named Server Traffic between Backend and Database transferring authentication data (like credentials, token, session-id, etc.)</t>
+  </si>
+  <si>
+    <t>Encryption of Communication Links</t>
+  </si>
+  <si>
+    <t>Apply transport layer encryption to the communication link.</t>
+  </si>
+  <si>
+    <t>unencrypted-communication@backend&gt;server-traffic@backend@database</t>
+  </si>
+  <si>
+    <t>CWE-311</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Assets</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named Backend</t>
+  </si>
+  <si>
+    <t>Encryption of Technical Asset</t>
+  </si>
+  <si>
+    <t>Apply encryption to the technical asset.</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@backend</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named Database</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@database</t>
+  </si>
+  <si>
+    <t>Accepted</t>
+  </si>
+  <si>
+    <t>Risk accepted as tolerable</t>
+  </si>
+  <si>
+    <t>2023-10-01</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Denial of Service</t>
+  </si>
+  <si>
+    <t>CWE-400</t>
+  </si>
+  <si>
+    <t>DoS-risky Access Across Trust-Boundary</t>
+  </si>
+  <si>
+    <t>Denial-of-Service risky access of Backend by Frontend via User Traffic</t>
+  </si>
+  <si>
+    <t>Anti-DoS Measures</t>
+  </si>
+  <si>
+    <t>Apply anti-DoS techniques like throttling and/or per-client load blocking with quotas. Also for maintenance access routes consider applying a VPN instead of public reachable interfaces. Generally applying redundancy on the targeted technical asset reduces the risk of DoS.</t>
+  </si>
+  <si>
+    <t>dos-risky-access-across-trust-boundary@backend@frontend@frontend&gt;user-traffic</t>
+  </si>
+  <si>
+    <t>Mixed Targets on Shared Runtime</t>
+  </si>
+  <si>
+    <t>Mixed Targets on Shared Runtime named EKS might enable attackers moving from one less valuable target to a more valuable one</t>
+  </si>
+  <si>
+    <t>Runtime Separation</t>
+  </si>
+  <si>
+    <t>Use separate runtime environments for running different target components or apply similar separation styles to prevent load- or breach-related problems originating from one more attacker-facing asset impacts also the other more critical rated backend/datastore assets.</t>
+  </si>
+  <si>
+    <t>mixed-targets-on-shared-runtime@eks</t>
+  </si>
+  <si>
     <t>CWE-89</t>
   </si>
   <si>
     <t>SQL/NoSQL-Injection</t>
   </si>
   <si>
-    <t>Server Traffic</t>
-  </si>
-  <si>
     <t>SQL/NoSQL-Injection risk at Backend against database Database via Server Traffic</t>
   </si>
   <si>
@@ -241,268 +514,10 @@
     <t>sql-nosql-injection@backend@database@backend&gt;server-traffic</t>
   </si>
   <si>
-    <t>CWE-501</t>
-  </si>
-  <si>
-    <t>Unguarded Access From Internet</t>
-  </si>
-  <si>
-    <t>Unguarded Access from Internet of Backend by Frontend via User Traffic</t>
-  </si>
-  <si>
-    <t>Encapsulation of Technical Asset</t>
-  </si>
-  <si>
-    <t>Encapsulate the asset behind a guarding service, application, or reverse-proxy. For admin maintenance a bastion-host should be used as a jump-server. For file transfer a store-and-forward-host should be used as an indirect file exchange platform.</t>
-  </si>
-  <si>
-    <t>unguarded-access-from-internet@backend@frontend@frontend&gt;user-traffic</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>CWE-502</t>
-  </si>
-  <si>
-    <t>Untrusted Deserialization</t>
-  </si>
-  <si>
-    <t>Untrusted Deserialization risk at Database</t>
-  </si>
-  <si>
-    <t>Prevention of Deserialization of Untrusted Data</t>
-  </si>
-  <si>
-    <t>Try to avoid the deserialization of untrusted data (even of data within the same trust-boundary as long as it is sent across a remote connection) in order to stay safe from Untrusted Deserialization vulnerabilities. Alternatively a strict whitelisting approach of the classes/types/values to deserialize might help as well. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>untrusted-deserialization@database</t>
-  </si>
-  <si>
-    <t>CWE-912</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Backend</t>
-  </si>
-  <si>
-    <t>Container Infrastructure Hardening</t>
-  </si>
-  <si>
-    <t>Apply hardening of all container infrastructures (see for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; and the &lt;i&gt;Docker Bench for Security&lt;/i&gt;). Use only trusted base images of the original vendors, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;i&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Regularly execute container image scans with tools checking the layers for vulnerable components.</t>
-  </si>
-  <si>
-    <t>Are recommendations from the linked cheat sheet and referenced ASVS/CSVS applied?</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@backend</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Database</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@database</t>
-  </si>
-  <si>
-    <t>Frontend</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Frontend</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@frontend</t>
-  </si>
-  <si>
-    <t>CWE-1127</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure in the threat model (referencing asset Backend as an example)</t>
-  </si>
-  <si>
-    <t>Build Pipeline Hardening</t>
-  </si>
-  <si>
-    <t>Include the build infrastructure in the model.</t>
-  </si>
-  <si>
-    <t>missing-build-infrastructure@backend</t>
-  </si>
-  <si>
-    <t>CWE-308</t>
-  </si>
-  <si>
-    <t>Missing Two-Factor Authentication (2FA)</t>
-  </si>
-  <si>
-    <t>Missing Two-Factor Authentication covering communication link User Traffic from Frontend to Backend</t>
-  </si>
-  <si>
-    <t>Authentication with Second Factor (2FA)</t>
-  </si>
-  <si>
-    <t>Apply an authentication method to the technical asset protecting highly sensitive data via two-factor authentication for human users.</t>
-  </si>
-  <si>
-    <t>missing-authentication-second-factor@frontend&gt;user-traffic@frontend@backend</t>
-  </si>
-  <si>
-    <t>Missing Vault Isolation</t>
-  </si>
-  <si>
-    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset AWS Secret Manager Vault against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
-  </si>
-  <si>
-    <t>Network Segmentation</t>
-  </si>
-  <si>
-    <t>Apply a network segmentation trust-boundary around the highly sensitive vault assets and their datastores.</t>
-  </si>
-  <si>
-    <t>missing-vault-isolation@aws-secret-manager-vault</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF) risk at Backend</t>
-  </si>
-  <si>
-    <t>Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Consider placing a Web Application Firewall (WAF) in front of the web-services and/or web-applications. For cloud environments many cloud providers offer pre-configured WAFs. Even reverse proxies can be enhances by a WAF component via ModSecurity plugins.</t>
-  </si>
-  <si>
-    <t>Is a Web Application Firewall (WAF) in place?</t>
-  </si>
-  <si>
-    <t>missing-waf@backend</t>
-  </si>
-  <si>
-    <t>Information Disclosure</t>
-  </si>
-  <si>
-    <t>CWE-918</t>
-  </si>
-  <si>
-    <t>Server-Side Request Forgery (SSRF)</t>
-  </si>
-  <si>
-    <t>Vault Access (backend)</t>
-  </si>
-  <si>
-    <t>Server-Side Request Forgery (SSRF) risk at Backend server-side web-requesting the target AWS Secret Manager Vault via Vault Access (backend)</t>
-  </si>
-  <si>
-    <t>SSRF Prevention</t>
-  </si>
-  <si>
-    <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>server-side-request-forgery@backend@aws-secret-manager-vault@backend&gt;vault-access-backend</t>
-  </si>
-  <si>
-    <t>CWE-319</t>
-  </si>
-  <si>
-    <t>Unencrypted Communication</t>
-  </si>
-  <si>
-    <t>Unencrypted Communication named Server Traffic between Backend and Database transferring authentication data (like credentials, token, session-id, etc.)</t>
-  </si>
-  <si>
-    <t>Encryption of Communication Links</t>
-  </si>
-  <si>
-    <t>Apply transport layer encryption to the communication link.</t>
-  </si>
-  <si>
-    <t>unencrypted-communication@backend&gt;server-traffic@backend@database</t>
-  </si>
-  <si>
-    <t>CWE-311</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Assets</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named Backend</t>
-  </si>
-  <si>
-    <t>Encryption of Technical Asset</t>
-  </si>
-  <si>
-    <t>Apply encryption to the technical asset.</t>
-  </si>
-  <si>
-    <t>unencrypted-asset@backend</t>
-  </si>
-  <si>
-    <t>Unencrypted Technical Asset named Database</t>
-  </si>
-  <si>
-    <t>unencrypted-asset@database</t>
-  </si>
-  <si>
-    <t>Accepted</t>
-  </si>
-  <si>
-    <t>Risk accepted as tolerable</t>
-  </si>
-  <si>
-    <t>2023-10-01</t>
-  </si>
-  <si>
-    <t>Ciro Bologna</t>
-  </si>
-  <si>
-    <t>XYZ-1234</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>Denial of Service</t>
-  </si>
-  <si>
-    <t>CWE-400</t>
-  </si>
-  <si>
-    <t>DoS-risky Access Across Trust-Boundary</t>
-  </si>
-  <si>
-    <t>Denial-of-Service risky access of Backend by Frontend via User Traffic</t>
-  </si>
-  <si>
-    <t>Anti-DoS Measures</t>
-  </si>
-  <si>
-    <t>Apply anti-DoS techniques like throttling and/or per-client load blocking with quotas. Also for maintenance access routes consider applying a VPN instead of public reachable interfaces. Generally applying redundancy on the targeted technical asset reduces the risk of DoS.</t>
-  </si>
-  <si>
-    <t>dos-risky-access-across-trust-boundary@backend@frontend@frontend&gt;user-traffic</t>
-  </si>
-  <si>
-    <t>Mixed Targets on Shared Runtime</t>
-  </si>
-  <si>
-    <t>Mixed Targets on Shared Runtime named EKS might enable attackers moving from one less valuable target to a more valuable one</t>
-  </si>
-  <si>
-    <t>Runtime Separation</t>
-  </si>
-  <si>
-    <t>Use separate runtime environments for running different target components or apply similar separation styles to prevent load- or breach-related problems originating from one more attacker-facing asset impacts also the other more critical rated backend/datastore assets.</t>
-  </si>
-  <si>
-    <t>mixed-targets-on-shared-runtime@eks</t>
+    <t>Mitigated</t>
+  </si>
+  <si>
+    <t>The backend is using hibernate and not manipulating SQL directly</t>
   </si>
 </sst>
 </file>
@@ -1330,13 +1345,21 @@
       <c r="O5" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="P5" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="18"/>
-      <c r="S5" s="18"/>
-      <c r="T5" s="17"/>
+      <c r="P5" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q5" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="S5" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T5" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="6" t="s">
@@ -1370,7 +1393,7 @@
         <v>100</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="L6" s="23" t="s">
         <v>61</v>
@@ -1382,61 +1405,69 @@
         <v>45</v>
       </c>
       <c r="O6" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="P6" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q6" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="P6" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="17"/>
+      <c r="R6" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="S6" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T6" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>67</v>
+        <v>37</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H7" s="5" t="s">
         <v>40</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
       <c r="J7" s="19">
         <v>100</v>
       </c>
       <c r="K7" s="20" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="L7" s="23" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="M7" s="23" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="N7" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O7" s="21" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="P7" s="11" t="s">
         <v>34</v>
@@ -1451,46 +1482,46 @@
         <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>21</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J8" s="19">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="K8" s="20" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
       <c r="L8" s="23" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="M8" s="23" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="N8" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O8" s="21" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>34</v>
@@ -1501,50 +1532,50 @@
       <c r="T8" s="17"/>
     </row>
     <row r="9">
-      <c r="A9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="D9" s="6" t="s">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I9" s="5" t="s">
+      <c r="E9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J9" s="19">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="K9" s="20" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="L9" s="23" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="M9" s="23" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="N9" s="23" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="O9" s="21" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>34</v>
@@ -1562,7 +1593,7 @@
         <v>47</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D10" s="8" t="s">
         <v>49</v>
@@ -1571,34 +1602,34 @@
         <v>50</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G10" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I10" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J10" s="19">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="K10" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="L10" s="23" t="s">
+        <v>88</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" s="23" t="s">
         <v>90</v>
       </c>
-      <c r="L10" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>92</v>
-      </c>
-      <c r="N10" s="23" t="s">
+      <c r="O10" s="21" t="s">
         <v>93</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>94</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>34</v>
@@ -1625,31 +1656,31 @@
         <v>50</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>27</v>
+        <v>94</v>
       </c>
       <c r="I11" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J11" s="19">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="K11" s="20" t="s">
         <v>95</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="N11" s="23" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="O11" s="21" t="s">
         <v>96</v>
@@ -1676,37 +1707,37 @@
         <v>49</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="G12" s="7" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="I12" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J12" s="19">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="N12" s="23" t="s">
-        <v>93</v>
+        <v>45</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>34</v>
@@ -1727,40 +1758,40 @@
         <v>22</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I13" s="7" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="J13" s="19">
         <v>100</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="N13" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>34</v>
@@ -1778,43 +1809,43 @@
         <v>47</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>106</v>
+        <v>51</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J14" s="19">
-        <v>100</v>
+        <v>69</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>34</v>
@@ -1832,10 +1863,10 @@
         <v>47</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>50</v>
@@ -1844,31 +1875,31 @@
         <v>51</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>59</v>
+        <v>40</v>
       </c>
       <c r="I15" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J15" s="19">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>34</v>
@@ -1889,40 +1920,40 @@
         <v>22</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>49</v>
+        <v>120</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>50</v>
+        <v>121</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>51</v>
+        <v>122</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>117</v>
+        <v>123</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>28</v>
+        <v>124</v>
       </c>
       <c r="J16" s="19">
         <v>100</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="L16" s="23" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="M16" s="23" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="N16" s="23" t="s">
-        <v>121</v>
+        <v>45</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>34</v>
@@ -1940,43 +1971,43 @@
         <v>47</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>22</v>
+        <v>78</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="G17" s="7" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="J17" s="19">
         <v>100</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="M17" s="23" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>130</v>
+        <v>135</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>34</v>
@@ -1994,43 +2025,43 @@
         <v>47</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>132</v>
+        <v>137</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I18" s="7" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="J18" s="19">
         <v>100</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>134</v>
+        <v>139</v>
       </c>
       <c r="M18" s="23" t="s">
-        <v>135</v>
+        <v>140</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>34</v>
@@ -2048,159 +2079,159 @@
         <v>47</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>81</v>
+        <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>138</v>
-      </c>
       <c r="H19" s="7" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J19" s="19">
-        <v>100</v>
+        <v>53</v>
       </c>
       <c r="K19" s="20" t="s">
+        <v>142</v>
+      </c>
+      <c r="L19" s="23" t="s">
         <v>139</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="M19" s="23" t="s">
         <v>140</v>
-      </c>
-      <c r="M19" s="23" t="s">
-        <v>141</v>
       </c>
       <c r="N19" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>142</v>
-      </c>
-      <c r="P19" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q19" s="20"/>
-      <c r="R19" s="18"/>
-      <c r="S19" s="18"/>
-      <c r="T19" s="17"/>
+        <v>143</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>144</v>
+      </c>
+      <c r="Q19" s="20" t="s">
+        <v>145</v>
+      </c>
+      <c r="R19" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="S19" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T19" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D20" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="E20" s="8" t="s">
+      <c r="C20" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="E20" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>138</v>
-      </c>
-      <c r="H20" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I20" s="7" t="s">
-        <v>28</v>
+      <c r="F20" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>41</v>
       </c>
       <c r="J20" s="19">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="L20" s="23" t="s">
-        <v>140</v>
+        <v>152</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="N20" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>144</v>
-      </c>
-      <c r="P20" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="Q20" s="20" t="s">
-        <v>146</v>
-      </c>
-      <c r="R20" s="18" t="s">
-        <v>147</v>
-      </c>
-      <c r="S20" s="18" t="s">
-        <v>148</v>
-      </c>
-      <c r="T20" s="17" t="s">
-        <v>149</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="P20" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q20" s="20"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="18"/>
+      <c r="T20" s="17"/>
     </row>
     <row r="21">
       <c r="A21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>47</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>151</v>
+        <v>36</v>
       </c>
       <c r="E21" s="10" t="s">
         <v>50</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>152</v>
+        <v>51</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H21" s="9" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J21" s="19">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="M21" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N21" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>34</v>
@@ -2211,58 +2242,66 @@
       <c r="T21" s="17"/>
     </row>
     <row r="22">
-      <c r="A22" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="B22" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="I22" s="9" t="s">
-        <v>28</v>
+      <c r="A22" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="C22" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D22" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>160</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="H22" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I22" s="22" t="s">
+        <v>131</v>
       </c>
       <c r="J22" s="19">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="K22" s="20" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="L22" s="23" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="M22" s="23" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="N22" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>162</v>
-      </c>
-      <c r="P22" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q22" s="20"/>
-      <c r="R22" s="18"/>
-      <c r="S22" s="18"/>
-      <c r="T22" s="17"/>
+        <v>165</v>
+      </c>
+      <c r="P22" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q22" s="20" t="s">
+        <v>167</v>
+      </c>
+      <c r="R22" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="S22" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T22" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
   </sheetData>
   <pageSetup orientation="landscape" paperSize="9"/>

</xml_diff>

<commit_message>
updating the threat model including devops pipeline
</commit_message>
<xml_diff>
--- a/risks.xlsx
+++ b/risks.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="275">
   <si>
     <t>Severity</t>
   </si>
@@ -193,214 +193,508 @@
     <t>Missing Hardening</t>
   </si>
   <si>
+    <t>Amazon EKS Container Platform</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at Amazon EKS Container Platform</t>
+  </si>
+  <si>
+    <t>System Hardening</t>
+  </si>
+  <si>
+    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
+  </si>
+  <si>
+    <t>missing-hardening@amazon-eks-container-platform</t>
+  </si>
+  <si>
+    <t>in Discussion</t>
+  </si>
+  <si>
+    <t>The hardening measures on the docker images are completed, the network ones in progress</t>
+  </si>
+  <si>
+    <t>2023-01-10</t>
+  </si>
+  <si>
+    <t>Ciro Bologna</t>
+  </si>
+  <si>
+    <t>XYZ-1234</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>missing-hardening@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>Missing Hardening risk at github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>missing-hardening@github-action-build-pipeline</t>
+  </si>
+  <si>
+    <t>Very Likely</t>
+  </si>
+  <si>
+    <t>CWE-501</t>
+  </si>
+  <si>
+    <t>Unguarded Access From Internet</t>
+  </si>
+  <si>
+    <t>Container Platform Traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Amazon EKS Container Platform by Development Client via Container Platform Traffic</t>
+  </si>
+  <si>
+    <t>Encapsulation of Technical Asset</t>
+  </si>
+  <si>
+    <t>Encapsulate the asset behind a guarding service, application, or reverse-proxy. For admin maintenance a bastion-host should be used as a jump-server. For file transfer a store-and-forward-host should be used as an indirect file exchange platform.</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@amazon-eks-container-platform@development-client@development-client&gt;container-platform-traffic</t>
+  </si>
+  <si>
+    <t>Artifact Registry Traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Nexus Artifact Registry by Development Client via Artifact Registry Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@nexus-artifact-registry@development-client@development-client&gt;artifact-registry-traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Nexus Artifact Registry by github action Build Pipeline via Artifact Registry Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@nexus-artifact-registry@github-action-build-pipeline@github-action-build-pipeline&gt;artifact-registry-traffic</t>
+  </si>
+  <si>
+    <t>github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>Sourcecode Repository Traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of github Sourcecode Repository by Development Client via Sourcecode Repository Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@github-sourcecode-repository@development-client@development-client&gt;sourcecode-repository-traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of github Sourcecode Repository by github action Build Pipeline via Sourcecode Repository Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@github-sourcecode-repository@github-action-build-pipeline@github-action-build-pipeline&gt;sourcecode-repository-traffic</t>
+  </si>
+  <si>
+    <t>Build Pipeline Traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of github action Build Pipeline by Development Client via Build Pipeline Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@github-action-build-pipeline@development-client@development-client&gt;build-pipeline-traffic</t>
+  </si>
+  <si>
+    <t>Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>Container Platform Pull</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Amazon ECR Container Registry by Amazon EKS Container Platform via Container Platform Pull</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@amazon-ecr-container-registry@amazon-eks-container-platform@amazon-eks-container-platform&gt;container-platform-pull</t>
+  </si>
+  <si>
+    <t>Container Registry Traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Amazon ECR Container Registry by Development Client via Container Registry Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@amazon-ecr-container-registry@development-client@development-client&gt;container-registry-traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Amazon ECR Container Registry by github action Build Pipeline via Container Registry Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@amazon-ecr-container-registry@github-action-build-pipeline@github-action-build-pipeline&gt;container-registry-traffic</t>
+  </si>
+  <si>
+    <t>Unguarded Access from Internet of Backend by Frontend via User Traffic</t>
+  </si>
+  <si>
+    <t>unguarded-access-from-internet@backend@frontend@frontend&gt;user-traffic</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>CWE-502</t>
+  </si>
+  <si>
+    <t>Untrusted Deserialization</t>
+  </si>
+  <si>
+    <t>Untrusted Deserialization risk at Database</t>
+  </si>
+  <si>
+    <t>Prevention of Deserialization of Untrusted Data</t>
+  </si>
+  <si>
+    <t>Try to avoid the deserialization of untrusted data (even of data within the same trust-boundary as long as it is sent across a remote connection) in order to stay safe from Untrusted Deserialization vulnerabilities. Alternatively a strict whitelisting approach of the classes/types/values to deserialize might help as well. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>untrusted-deserialization@database</t>
+  </si>
+  <si>
+    <t>Information Disclosure</t>
+  </si>
+  <si>
+    <t>CWE-200</t>
+  </si>
+  <si>
+    <t>Accidental Secret Leak</t>
+  </si>
+  <si>
+    <t>Accidental Secret Leak risk at Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>Build Pipeline Hardening</t>
+  </si>
+  <si>
+    <t>Establish measures preventing accidental check-in or package-in of secrets into sourcecode repositories and artifact registries. This starts by using good .gitignore and .dockerignore files, but does not stop there. See for example tools like &lt;i&gt;"git-secrets" or "Talisman"&lt;/i&gt; to have check-in preventive measures for secrets. Consider also to regularly scan your repositories for secrets accidentally checked-in using scanning tools like &lt;i&gt;"gitleaks" or "gitrob"&lt;/i&gt;.</t>
+  </si>
+  <si>
+    <t>accidental-secret-leak@amazon-ecr-container-registry</t>
+  </si>
+  <si>
+    <t>Accidental Secret Leak risk at Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>accidental-secret-leak@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Accidental Secret Leak risk at github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>accidental-secret-leak@github-sourcecode-repository</t>
+  </si>
+  <si>
+    <t>CWE-912</t>
+  </si>
+  <si>
+    <t>Code Backdooring</t>
+  </si>
+  <si>
+    <t>Code Backdooring risk at Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>Reduce the attack surface of backdooring the build pipeline by not directly exposing the build pipeline components on the public internet and also not exposing it in front of unmanaged (out-of-scope) developer clients.Also consider the use of code signing to prevent code modifications.</t>
+  </si>
+  <si>
+    <t>code-backdooring@amazon-ecr-container-registry</t>
+  </si>
+  <si>
+    <t>Code Backdooring risk at Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>code-backdooring@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Code Backdooring risk at github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>code-backdooring@github-sourcecode-repository</t>
+  </si>
+  <si>
+    <t>Code Backdooring risk at github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>code-backdooring@github-action-build-pipeline</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Backend</t>
+  </si>
+  <si>
+    <t>Container Infrastructure Hardening</t>
+  </si>
+  <si>
+    <t>Apply hardening of all container infrastructures (see for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; and the &lt;i&gt;Docker Bench for Security&lt;/i&gt;). Use only trusted base images of the original vendors, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;i&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Regularly execute container image scans with tools checking the layers for vulnerable components.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS/CSVS applied?</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@backend</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Database</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@database</t>
+  </si>
+  <si>
+    <t>Frontend</t>
+  </si>
+  <si>
+    <t>Container Base Image Backdooring risk at Frontend</t>
+  </si>
+  <si>
+    <t>container-baseimage-backdooring@frontend</t>
+  </si>
+  <si>
+    <t>Container Platform Escape</t>
+  </si>
+  <si>
+    <t>Container Platform Escape risk at Amazon EKS Container Platform</t>
+  </si>
+  <si>
+    <t>Apply hardening of all container infrastructures. &lt;p&gt;See for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; as well as the &lt;i&gt;Docker Bench for Security&lt;/i&gt; ( &lt;a href="https://github.com/docker/docker-bench-security"&gt;https://github.com/docker/docker-bench-security&lt;/a&gt; ) or &lt;i&gt;InSpec Checks for Docker and Kubernetes&lt;/i&gt; ( &lt;a href="https://github.com/dev-sec/cis-kubernetes-benchmark"&gt;https://github.com/dev-sec/cis-docker-benchmark&lt;/a&gt; and &lt;a href="https://github.com/dev-sec/cis-kubernetes-benchmark"&gt;https://github.com/dev-sec/cis-kubernetes-benchmark&lt;/a&gt; ). Use only trusted base images, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;b&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Apply namespace isolation and nod affinity to separate pods from each other in terms of access and nodes the same style as you separate data.</t>
+  </si>
+  <si>
+    <t>Are recommendations from the linked cheat sheet and referenced ASVS or CSVS chapter applied?</t>
+  </si>
+  <si>
+    <t>container-platform-escape@amazon-eks-container-platform</t>
+  </si>
+  <si>
+    <t>Spoofing</t>
+  </si>
+  <si>
+    <t>CWE-287</t>
+  </si>
+  <si>
+    <t>Missing Identity Store</t>
+  </si>
+  <si>
+    <t>Missing Identity Store in the threat model (referencing asset github Sourcecode Repository as an example)</t>
+  </si>
+  <si>
+    <t>Identity Store</t>
+  </si>
+  <si>
+    <t>Include an identity store in the model if the application has a login.</t>
+  </si>
+  <si>
+    <t>missing-identity-store@github-sourcecode-repository</t>
+  </si>
+  <si>
+    <t>Missing Network Segmentation</t>
+  </si>
+  <si>
+    <t>Missing Network Segmentation to further encapsulate and protect Amazon EKS Container Platform against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>Network Segmentation</t>
+  </si>
+  <si>
+    <t>Apply a network segmentation trust-boundary around the highly sensitive assets and/or datastores.</t>
+  </si>
+  <si>
+    <t>missing-network-segmentation@amazon-eks-container-platform</t>
+  </si>
+  <si>
+    <t>Missing Network Segmentation to further encapsulate and protect Nexus Artifact Registry against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>missing-network-segmentation@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Missing Network Segmentation to further encapsulate and protect github action Build Pipeline against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>missing-network-segmentation@github-action-build-pipeline</t>
+  </si>
+  <si>
+    <t>CWE-308</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication (2FA)</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link Artifact Registry Traffic from Development Client to Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>Authentication with Second Factor (2FA)</t>
+  </si>
+  <si>
+    <t>Apply an authentication method to the technical asset protecting highly sensitive data via two-factor authentication for human users.</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@development-client&gt;artifact-registry-traffic@development-client@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link Build Pipeline Traffic from Development Client to github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@development-client&gt;build-pipeline-traffic@development-client@github-action-build-pipeline</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link Container Platform Traffic from Development Client to Amazon EKS Container Platform</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@development-client&gt;container-platform-traffic@development-client@amazon-eks-container-platform</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link Container Registry Traffic from Development Client to Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@development-client&gt;container-registry-traffic@development-client@amazon-ecr-container-registry</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link Sourcecode Repository Traffic from Development Client to github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@development-client&gt;sourcecode-repository-traffic@development-client@github-sourcecode-repository</t>
+  </si>
+  <si>
+    <t>Missing Two-Factor Authentication covering communication link User Traffic from Frontend to Backend</t>
+  </si>
+  <si>
+    <t>missing-authentication-second-factor@frontend&gt;user-traffic@frontend@backend</t>
+  </si>
+  <si>
+    <t>Missing Vault Isolation</t>
+  </si>
+  <si>
     <t>AWS Secret Manager Vault</t>
   </si>
   <si>
-    <t>Missing Hardening risk at AWS Secret Manager Vault</t>
-  </si>
-  <si>
-    <t>System Hardening</t>
-  </si>
-  <si>
-    <t>Try to apply all hardening best practices (like CIS benchmarks, OWASP recommendations, vendor recommendations, DevSec Hardening Framework, DBSAT for Oracle databases, and others).</t>
-  </si>
-  <si>
-    <t>missing-hardening@aws-secret-manager-vault</t>
-  </si>
-  <si>
-    <t>in Discussion</t>
-  </si>
-  <si>
-    <t>The hardening measures on the docker images are completed, the network ones in progress</t>
-  </si>
-  <si>
-    <t>2023-01-10</t>
-  </si>
-  <si>
-    <t>Ciro Bologna</t>
-  </si>
-  <si>
-    <t>XYZ-1234</t>
-  </si>
-  <si>
-    <t>Missing Hardening risk at Backend</t>
-  </si>
-  <si>
-    <t>missing-hardening@backend</t>
-  </si>
-  <si>
-    <t>Very Likely</t>
-  </si>
-  <si>
-    <t>CWE-501</t>
-  </si>
-  <si>
-    <t>Unguarded Access From Internet</t>
-  </si>
-  <si>
-    <t>Unguarded Access from Internet of Backend by Frontend via User Traffic</t>
-  </si>
-  <si>
-    <t>Encapsulation of Technical Asset</t>
-  </si>
-  <si>
-    <t>Encapsulate the asset behind a guarding service, application, or reverse-proxy. For admin maintenance a bastion-host should be used as a jump-server. For file transfer a store-and-forward-host should be used as an indirect file exchange platform.</t>
-  </si>
-  <si>
-    <t>unguarded-access-from-internet@backend@frontend@frontend&gt;user-traffic</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>CWE-502</t>
-  </si>
-  <si>
-    <t>Untrusted Deserialization</t>
-  </si>
-  <si>
-    <t>Untrusted Deserialization risk at Database</t>
-  </si>
-  <si>
-    <t>Prevention of Deserialization of Untrusted Data</t>
-  </si>
-  <si>
-    <t>Try to avoid the deserialization of untrusted data (even of data within the same trust-boundary as long as it is sent across a remote connection) in order to stay safe from Untrusted Deserialization vulnerabilities. Alternatively a strict whitelisting approach of the classes/types/values to deserialize might help as well. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>untrusted-deserialization@database</t>
-  </si>
-  <si>
-    <t>CWE-912</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Backend</t>
-  </si>
-  <si>
-    <t>Container Infrastructure Hardening</t>
-  </si>
-  <si>
-    <t>Apply hardening of all container infrastructures (see for example the &lt;i&gt;CIS-Benchmarks for Docker and Kubernetes&lt;/i&gt; and the &lt;i&gt;Docker Bench for Security&lt;/i&gt;). Use only trusted base images of the original vendors, verify digital signatures and apply image creation best practices. Also consider using Google's &lt;i&gt;Distroless&lt;/i&gt; base images or otherwise very small base images. Regularly execute container image scans with tools checking the layers for vulnerable components.</t>
-  </si>
-  <si>
-    <t>Are recommendations from the linked cheat sheet and referenced ASVS/CSVS applied?</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@backend</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Database</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@database</t>
-  </si>
-  <si>
-    <t>Frontend</t>
-  </si>
-  <si>
-    <t>Container Base Image Backdooring risk at Frontend</t>
-  </si>
-  <si>
-    <t>container-baseimage-backdooring@frontend</t>
+    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset AWS Secret Manager Vault against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
+  </si>
+  <si>
+    <t>Apply a network segmentation trust-boundary around the highly sensitive vault assets and their datastores.</t>
+  </si>
+  <si>
+    <t>missing-vault-isolation@aws-secret-manager-vault</t>
+  </si>
+  <si>
+    <t>Missing Web Application Firewall (WAF)</t>
+  </si>
+  <si>
+    <t>Missing Web Application Firewall (WAF) risk at Backend</t>
+  </si>
+  <si>
+    <t>Web Application Firewall (WAF)</t>
+  </si>
+  <si>
+    <t>Consider placing a Web Application Firewall (WAF) in front of the web-services and/or web-applications. For cloud environments many cloud providers offer pre-configured WAFs. Even reverse proxies can be enhances by a WAF component via ModSecurity plugins.</t>
+  </si>
+  <si>
+    <t>Is a Web Application Firewall (WAF) in place?</t>
+  </si>
+  <si>
+    <t>missing-waf@backend</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t>CWE-918</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF)</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at Amazon EKS Container Platform server-side web-requesting the target Amazon ECR Container Registry via Container Platform Pull</t>
+  </si>
+  <si>
+    <t>SSRF Prevention</t>
+  </si>
+  <si>
+    <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@amazon-eks-container-platform@amazon-ecr-container-registry@amazon-eks-container-platform&gt;container-platform-pull</t>
+  </si>
+  <si>
+    <t>Vault Access (backend)</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at Backend server-side web-requesting the target AWS Secret Manager Vault via Vault Access (backend)</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@backend@aws-secret-manager-vault@backend&gt;vault-access-backend</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at github action Build Pipeline server-side web-requesting the target Amazon ECR Container Registry via Container Registry Traffic</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@github-action-build-pipeline@amazon-ecr-container-registry@github-action-build-pipeline&gt;container-registry-traffic</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at github action Build Pipeline server-side web-requesting the target Nexus Artifact Registry via Artifact Registry Traffic</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@github-action-build-pipeline@nexus-artifact-registry@github-action-build-pipeline&gt;artifact-registry-traffic</t>
+  </si>
+  <si>
+    <t>Server-Side Request Forgery (SSRF) risk at github action Build Pipeline server-side web-requesting the target github Sourcecode Repository via Sourcecode Repository Traffic</t>
+  </si>
+  <si>
+    <t>server-side-request-forgery@github-action-build-pipeline@github-sourcecode-repository@github-action-build-pipeline&gt;sourcecode-repository-traffic</t>
   </si>
   <si>
     <t>CWE-1127</t>
   </si>
   <si>
-    <t>Missing Build Infrastructure</t>
-  </si>
-  <si>
-    <t>Missing Build Infrastructure in the threat model (referencing asset Backend as an example)</t>
-  </si>
-  <si>
-    <t>Build Pipeline Hardening</t>
-  </si>
-  <si>
-    <t>Include the build infrastructure in the model.</t>
-  </si>
-  <si>
-    <t>missing-build-infrastructure@backend</t>
-  </si>
-  <si>
-    <t>CWE-308</t>
-  </si>
-  <si>
-    <t>Missing Two-Factor Authentication (2FA)</t>
-  </si>
-  <si>
-    <t>Missing Two-Factor Authentication covering communication link User Traffic from Frontend to Backend</t>
-  </si>
-  <si>
-    <t>Authentication with Second Factor (2FA)</t>
-  </si>
-  <si>
-    <t>Apply an authentication method to the technical asset protecting highly sensitive data via two-factor authentication for human users.</t>
-  </si>
-  <si>
-    <t>missing-authentication-second-factor@frontend&gt;user-traffic@frontend@backend</t>
-  </si>
-  <si>
-    <t>Missing Vault Isolation</t>
-  </si>
-  <si>
-    <t>Missing Vault Isolation to further encapsulate and protect vault-related asset AWS Secret Manager Vault against unrelated lower protected assets in the same network segment, which might be easier to compromise by attackers</t>
-  </si>
-  <si>
-    <t>Network Segmentation</t>
-  </si>
-  <si>
-    <t>Apply a network segmentation trust-boundary around the highly sensitive vault assets and their datastores.</t>
-  </si>
-  <si>
-    <t>missing-vault-isolation@aws-secret-manager-vault</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Missing Web Application Firewall (WAF) risk at Backend</t>
-  </si>
-  <si>
-    <t>Web Application Firewall (WAF)</t>
-  </si>
-  <si>
-    <t>Consider placing a Web Application Firewall (WAF) in front of the web-services and/or web-applications. For cloud environments many cloud providers offer pre-configured WAFs. Even reverse proxies can be enhances by a WAF component via ModSecurity plugins.</t>
-  </si>
-  <si>
-    <t>Is a Web Application Firewall (WAF) in place?</t>
-  </si>
-  <si>
-    <t>missing-waf@backend</t>
-  </si>
-  <si>
-    <t>Information Disclosure</t>
-  </si>
-  <si>
-    <t>Development</t>
-  </si>
-  <si>
-    <t>CWE-918</t>
-  </si>
-  <si>
-    <t>Server-Side Request Forgery (SSRF)</t>
-  </si>
-  <si>
-    <t>Vault Access (backend)</t>
-  </si>
-  <si>
-    <t>Server-Side Request Forgery (SSRF) risk at Backend server-side web-requesting the target AWS Secret Manager Vault via Vault Access (backend)</t>
-  </si>
-  <si>
-    <t>SSRF Prevention</t>
-  </si>
-  <si>
-    <t>Try to avoid constructing the outgoing target URL with caller controllable values. Alternatively use a mapping (whitelist) when accessing outgoing URLs instead of creating them including caller controllable values. When a third-party product is used instead of custom developed software, check if the product applies the proper mitigation and ensure a reasonable patch-level.</t>
-  </si>
-  <si>
-    <t>server-side-request-forgery@backend@aws-secret-manager-vault@backend&gt;vault-access-backend</t>
+    <t>Unchecked Deployment</t>
+  </si>
+  <si>
+    <t>Development Client</t>
+  </si>
+  <si>
+    <t>Unchecked Deployment risk at Development Client</t>
+  </si>
+  <si>
+    <t>Apply DevSecOps best-practices and use scanning tools to identify vulnerabilities in source- or byte-code,dependencies, container layers, and optionally also via dynamic scans against running test systems.</t>
+  </si>
+  <si>
+    <t>unchecked-deployment@development-client</t>
+  </si>
+  <si>
+    <t>Unchecked Deployment risk at github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>unchecked-deployment@github-action-build-pipeline</t>
+  </si>
+  <si>
+    <t>Unchecked Deployment risk at Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>unchecked-deployment@amazon-ecr-container-registry</t>
+  </si>
+  <si>
+    <t>Unchecked Deployment risk at Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>unchecked-deployment@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Unchecked Deployment risk at github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>unchecked-deployment@github-sourcecode-repository</t>
   </si>
   <si>
     <t>CWE-319</t>
@@ -430,18 +724,48 @@
     <t>Unencrypted Technical Assets</t>
   </si>
   <si>
+    <t>Unencrypted Technical Asset named Amazon EKS Container Platform</t>
+  </si>
+  <si>
+    <t>Encryption of Technical Asset</t>
+  </si>
+  <si>
+    <t>Apply encryption to the technical asset.</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@amazon-eks-container-platform</t>
+  </si>
+  <si>
     <t>Unencrypted Technical Asset named Backend</t>
   </si>
   <si>
-    <t>Encryption of Technical Asset</t>
-  </si>
-  <si>
-    <t>Apply encryption to the technical asset.</t>
-  </si>
-  <si>
     <t>unencrypted-asset@backend</t>
   </si>
   <si>
+    <t>Unencrypted Technical Asset named Amazon ECR Container Registry</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@amazon-ecr-container-registry</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named Nexus Artifact Registry</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@nexus-artifact-registry</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named github Sourcecode Repository</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@github-sourcecode-repository</t>
+  </si>
+  <si>
+    <t>Unencrypted Technical Asset named github action Build Pipeline</t>
+  </si>
+  <si>
+    <t>unencrypted-asset@github-action-build-pipeline</t>
+  </si>
+  <si>
     <t>Unencrypted Technical Asset named Database</t>
   </si>
   <si>
@@ -455,9 +779,6 @@
   </si>
   <si>
     <t>2023-10-01</t>
-  </si>
-  <si>
-    <t>Low</t>
   </si>
   <si>
     <t>Denial of Service</t>
@@ -1166,7 +1487,7 @@
         <v>28</v>
       </c>
       <c r="J2" s="19">
-        <v>53</v>
+        <v>28</v>
       </c>
       <c r="K2" s="20" t="s">
         <v>29</v>
@@ -1220,7 +1541,7 @@
         <v>41</v>
       </c>
       <c r="J3" s="19">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="K3" s="20" t="s">
         <v>42</v>
@@ -1328,7 +1649,7 @@
         <v>28</v>
       </c>
       <c r="J5" s="19">
-        <v>69</v>
+        <v>100</v>
       </c>
       <c r="K5" s="20" t="s">
         <v>60</v>
@@ -1362,38 +1683,38 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" s="6" t="s">
+      <c r="A6" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="6" t="s">
+      <c r="C6" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="6" t="s">
+      <c r="F6" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" s="5" t="s">
+      <c r="H6" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J6" s="19">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="K6" s="20" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L6" s="23" t="s">
         <v>61</v>
@@ -1405,7 +1726,7 @@
         <v>45</v>
       </c>
       <c r="O6" s="21" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="P6" s="15" t="s">
         <v>64</v>
@@ -1424,104 +1745,112 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" s="5" t="s">
+      <c r="A7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="H7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="I7" s="5" t="s">
-        <v>41</v>
+      <c r="I7" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="J7" s="19">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="K7" s="20" t="s">
         <v>74</v>
       </c>
       <c r="L7" s="23" t="s">
+        <v>61</v>
+      </c>
+      <c r="M7" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="N7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O7" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="M7" s="23" t="s">
-        <v>76</v>
-      </c>
-      <c r="N7" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="O7" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="P7" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="18"/>
-      <c r="S7" s="18"/>
-      <c r="T7" s="17"/>
+      <c r="P7" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q7" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="R7" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="S7" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T7" s="17" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>78</v>
+        <v>22</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>37</v>
       </c>
       <c r="F8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="I8" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="G8" s="5" t="s">
+      <c r="J8" s="19">
+        <v>100</v>
+      </c>
+      <c r="K8" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="H8" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="19">
-        <v>53</v>
-      </c>
-      <c r="K8" s="20" t="s">
+      <c r="L8" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="M8" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="M8" s="23" t="s">
+      <c r="N8" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O8" s="21" t="s">
         <v>83</v>
-      </c>
-      <c r="N8" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>84</v>
       </c>
       <c r="P8" s="11" t="s">
         <v>34</v>
@@ -1532,50 +1861,50 @@
       <c r="T8" s="17"/>
     </row>
     <row r="9">
-      <c r="A9" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F9" s="8" t="s">
+      <c r="H9" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="J9" s="19">
+        <v>59</v>
+      </c>
+      <c r="K9" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="G9" s="7" t="s">
+      <c r="L9" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M9" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="N9" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O9" s="21" t="s">
         <v>86</v>
-      </c>
-      <c r="H9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I9" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="J9" s="19">
-        <v>100</v>
-      </c>
-      <c r="K9" s="20" t="s">
-        <v>87</v>
-      </c>
-      <c r="L9" s="23" t="s">
-        <v>88</v>
-      </c>
-      <c r="M9" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="N9" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="O9" s="21" t="s">
-        <v>91</v>
       </c>
       <c r="P9" s="11" t="s">
         <v>34</v>
@@ -1586,50 +1915,50 @@
       <c r="T9" s="17"/>
     </row>
     <row r="10">
-      <c r="A10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E10" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="I10" s="7" t="s">
-        <v>28</v>
+      <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="J10" s="19">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="K10" s="20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="L10" s="23" t="s">
+        <v>81</v>
+      </c>
+      <c r="M10" s="23" t="s">
+        <v>82</v>
+      </c>
+      <c r="N10" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O10" s="21" t="s">
         <v>88</v>
-      </c>
-      <c r="M10" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="N10" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>93</v>
       </c>
       <c r="P10" s="11" t="s">
         <v>34</v>
@@ -1640,50 +1969,50 @@
       <c r="T10" s="17"/>
     </row>
     <row r="11">
-      <c r="A11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="H11" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="I11" s="7" t="s">
-        <v>28</v>
+      <c r="A11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J11" s="19">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="K11" s="20" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="M11" s="23" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="N11" s="23" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="P11" s="11" t="s">
         <v>34</v>
@@ -1694,50 +2023,50 @@
       <c r="T11" s="17"/>
     </row>
     <row r="12">
-      <c r="A12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="8" t="s">
+      <c r="A12" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H12" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I12" s="7" t="s">
-        <v>28</v>
+      <c r="F12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="J12" s="19">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="K12" s="20" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>100</v>
+        <v>81</v>
       </c>
       <c r="M12" s="23" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="N12" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="P12" s="11" t="s">
         <v>34</v>
@@ -1748,50 +2077,50 @@
       <c r="T12" s="17"/>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="8" t="s">
+      <c r="A13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="H13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I13" s="7" t="s">
-        <v>41</v>
+      <c r="E13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="J13" s="19">
-        <v>100</v>
+        <v>82</v>
       </c>
       <c r="K13" s="20" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>106</v>
+        <v>81</v>
       </c>
       <c r="M13" s="23" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
       <c r="N13" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="P13" s="11" t="s">
         <v>34</v>
@@ -1806,46 +2135,46 @@
         <v>22</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="D14" s="8" t="s">
         <v>36</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>59</v>
+        <v>98</v>
       </c>
       <c r="I14" s="7" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="J14" s="19">
-        <v>69</v>
+        <v>29</v>
       </c>
       <c r="K14" s="20" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>111</v>
+        <v>81</v>
       </c>
       <c r="M14" s="23" t="s">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="N14" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O14" s="21" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="P14" s="11" t="s">
         <v>34</v>
@@ -1860,46 +2189,46 @@
         <v>22</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="I15" s="7" t="s">
-        <v>28</v>
+        <v>102</v>
       </c>
       <c r="J15" s="19">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="K15" s="20" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>116</v>
+        <v>81</v>
       </c>
       <c r="M15" s="23" t="s">
-        <v>117</v>
+        <v>82</v>
       </c>
       <c r="N15" s="23" t="s">
-        <v>118</v>
+        <v>45</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="P15" s="11" t="s">
         <v>34</v>
@@ -1914,46 +2243,46 @@
         <v>22</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>22</v>
+        <v>69</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>120</v>
+        <v>36</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>121</v>
+        <v>37</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>122</v>
+        <v>77</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>123</v>
+        <v>78</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>40</v>
+        <v>98</v>
       </c>
       <c r="I16" s="7" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="J16" s="19">
-        <v>100</v>
+        <v>29</v>
       </c>
       <c r="K16" s="20" t="s">
-        <v>125</v>
+        <v>105</v>
       </c>
       <c r="L16" s="23" t="s">
-        <v>126</v>
+        <v>81</v>
       </c>
       <c r="M16" s="23" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="N16" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="P16" s="11" t="s">
         <v>34</v>
@@ -1968,46 +2297,46 @@
         <v>22</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>47</v>
+        <v>76</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>130</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>40</v>
       </c>
       <c r="I17" s="7" t="s">
-        <v>131</v>
+        <v>41</v>
       </c>
       <c r="J17" s="19">
-        <v>100</v>
+        <v>36</v>
       </c>
       <c r="K17" s="20" t="s">
-        <v>132</v>
+        <v>107</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>133</v>
+        <v>81</v>
       </c>
       <c r="M17" s="23" t="s">
-        <v>134</v>
+        <v>82</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="P17" s="11" t="s">
         <v>34</v>
@@ -2018,50 +2347,50 @@
       <c r="T17" s="17"/>
     </row>
     <row r="18">
-      <c r="A18" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>136</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H18" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="I18" s="7" t="s">
+      <c r="A18" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>28</v>
       </c>
       <c r="J18" s="19">
-        <v>100</v>
+        <v>28</v>
       </c>
       <c r="K18" s="20" t="s">
-        <v>138</v>
+        <v>112</v>
       </c>
       <c r="L18" s="23" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="M18" s="23" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="N18" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>141</v>
+        <v>115</v>
       </c>
       <c r="P18" s="11" t="s">
         <v>34</v>
@@ -2082,102 +2411,94 @@
         <v>22</v>
       </c>
       <c r="D19" s="8" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>50</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>136</v>
+        <v>117</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>137</v>
+        <v>118</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>27</v>
+        <v>98</v>
       </c>
       <c r="I19" s="7" t="s">
         <v>28</v>
       </c>
       <c r="J19" s="19">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="K19" s="20" t="s">
-        <v>142</v>
+        <v>119</v>
       </c>
       <c r="L19" s="23" t="s">
-        <v>139</v>
+        <v>120</v>
       </c>
       <c r="M19" s="23" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="N19" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O19" s="21" t="s">
-        <v>143</v>
-      </c>
-      <c r="P19" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="Q19" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="R19" s="18" t="s">
-        <v>146</v>
-      </c>
-      <c r="S19" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="T19" s="17" t="s">
-        <v>68</v>
-      </c>
+        <v>122</v>
+      </c>
+      <c r="P19" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q19" s="20"/>
+      <c r="R19" s="18"/>
+      <c r="S19" s="18"/>
+      <c r="T19" s="17"/>
     </row>
     <row r="20">
-      <c r="A20" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B20" s="10" t="s">
+      <c r="A20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="E20" s="10" t="s">
+      <c r="C20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F20" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="H20" s="9" t="s">
-        <v>40</v>
-      </c>
-      <c r="I20" s="9" t="s">
-        <v>41</v>
+      <c r="F20" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>28</v>
       </c>
       <c r="J20" s="19">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="K20" s="20" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="L20" s="23" t="s">
-        <v>152</v>
+        <v>120</v>
       </c>
       <c r="M20" s="23" t="s">
-        <v>153</v>
+        <v>121</v>
       </c>
       <c r="N20" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>154</v>
+        <v>124</v>
       </c>
       <c r="P20" s="11" t="s">
         <v>34</v>
@@ -2188,50 +2509,50 @@
       <c r="T20" s="17"/>
     </row>
     <row r="21">
-      <c r="A21" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="B21" s="10" t="s">
+      <c r="A21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="C21" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="C21" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="F21" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="H21" s="9" t="s">
+      <c r="F21" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I21" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I21" s="9" t="s">
-        <v>28</v>
-      </c>
       <c r="J21" s="19">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="K21" s="20" t="s">
-        <v>156</v>
+        <v>125</v>
       </c>
       <c r="L21" s="23" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="M21" s="23" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="N21" s="23" t="s">
         <v>45</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>159</v>
+        <v>126</v>
       </c>
       <c r="P21" s="11" t="s">
         <v>34</v>
@@ -2242,64 +2563,2232 @@
       <c r="T21" s="17"/>
     </row>
     <row r="22">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="19">
+        <v>29</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="L22" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M22" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O22" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="P22" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q22" s="20"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="17"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J23" s="19">
+        <v>59</v>
+      </c>
+      <c r="K23" s="20" t="s">
+        <v>132</v>
+      </c>
+      <c r="L23" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M23" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="N23" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="P23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q23" s="20"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="17"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D24" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J24" s="19">
+        <v>43</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="L24" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M24" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="N24" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>135</v>
+      </c>
+      <c r="P24" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q24" s="20"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="18"/>
+      <c r="T24" s="17"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J25" s="19">
+        <v>82</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>136</v>
+      </c>
+      <c r="L25" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M25" s="23" t="s">
+        <v>130</v>
+      </c>
+      <c r="N25" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O25" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="P25" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q25" s="20"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="18"/>
+      <c r="T25" s="17"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D26" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H26" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I26" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J26" s="19">
+        <v>36</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="L26" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="M26" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="N26" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="O26" s="21" t="s">
+        <v>143</v>
+      </c>
+      <c r="P26" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q26" s="20"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="17"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J27" s="19">
+        <v>28</v>
+      </c>
+      <c r="K27" s="20" t="s">
+        <v>144</v>
+      </c>
+      <c r="L27" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="M27" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="N27" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="O27" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="P27" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q27" s="20"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="17"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F28" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="I28" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J28" s="19">
+        <v>19</v>
+      </c>
+      <c r="K28" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="L28" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="M28" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="N28" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="O28" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="P28" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q28" s="20"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="17"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F29" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J29" s="19">
+        <v>100</v>
+      </c>
+      <c r="K29" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="L29" s="23" t="s">
+        <v>140</v>
+      </c>
+      <c r="M29" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="N29" s="23" t="s">
+        <v>152</v>
+      </c>
+      <c r="O29" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="P29" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q29" s="20"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="17"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G30" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="H30" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I30" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J30" s="19">
+        <v>43</v>
+      </c>
+      <c r="K30" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="L30" s="23" t="s">
+        <v>158</v>
+      </c>
+      <c r="M30" s="23" t="s">
+        <v>159</v>
+      </c>
+      <c r="N30" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O30" s="21" t="s">
+        <v>160</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q30" s="20"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="17"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I31" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J31" s="19">
+        <v>100</v>
+      </c>
+      <c r="K31" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="L31" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M31" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="N31" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>165</v>
+      </c>
+      <c r="P31" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q31" s="20"/>
+      <c r="R31" s="18"/>
+      <c r="S31" s="18"/>
+      <c r="T31" s="17"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J32" s="19">
+        <v>59</v>
+      </c>
+      <c r="K32" s="20" t="s">
+        <v>166</v>
+      </c>
+      <c r="L32" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M32" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="N32" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O32" s="21" t="s">
+        <v>167</v>
+      </c>
+      <c r="P32" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q32" s="20"/>
+      <c r="R32" s="18"/>
+      <c r="S32" s="18"/>
+      <c r="T32" s="17"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J33" s="19">
+        <v>82</v>
+      </c>
+      <c r="K33" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="L33" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M33" s="23" t="s">
+        <v>164</v>
+      </c>
+      <c r="N33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O33" s="21" t="s">
+        <v>169</v>
+      </c>
+      <c r="P33" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q33" s="20"/>
+      <c r="R33" s="18"/>
+      <c r="S33" s="18"/>
+      <c r="T33" s="17"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I34" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="19">
+        <v>59</v>
+      </c>
+      <c r="K34" s="20" t="s">
+        <v>172</v>
+      </c>
+      <c r="L34" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M34" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N34" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O34" s="21" t="s">
+        <v>175</v>
+      </c>
+      <c r="P34" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q34" s="20"/>
+      <c r="R34" s="18"/>
+      <c r="S34" s="18"/>
+      <c r="T34" s="17"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I35" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="J35" s="19">
+        <v>82</v>
+      </c>
+      <c r="K35" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="L35" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M35" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O35" s="21" t="s">
+        <v>177</v>
+      </c>
+      <c r="P35" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q35" s="20"/>
+      <c r="R35" s="18"/>
+      <c r="S35" s="18"/>
+      <c r="T35" s="17"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G36" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H36" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I36" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="J36" s="19">
+        <v>100</v>
+      </c>
+      <c r="K36" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="L36" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M36" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N36" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O36" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="P36" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q36" s="20"/>
+      <c r="R36" s="18"/>
+      <c r="S36" s="18"/>
+      <c r="T36" s="17"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I37" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J37" s="19">
+        <v>29</v>
+      </c>
+      <c r="K37" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="L37" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M37" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N37" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O37" s="21" t="s">
+        <v>181</v>
+      </c>
+      <c r="P37" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q37" s="20"/>
+      <c r="R37" s="18"/>
+      <c r="S37" s="18"/>
+      <c r="T37" s="17"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F38" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G38" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H38" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J38" s="19">
+        <v>43</v>
+      </c>
+      <c r="K38" s="20" t="s">
+        <v>182</v>
+      </c>
+      <c r="L38" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M38" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N38" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O38" s="21" t="s">
+        <v>183</v>
+      </c>
+      <c r="P38" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q38" s="20"/>
+      <c r="R38" s="18"/>
+      <c r="S38" s="18"/>
+      <c r="T38" s="17"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="J39" s="19">
+        <v>36</v>
+      </c>
+      <c r="K39" s="20" t="s">
+        <v>184</v>
+      </c>
+      <c r="L39" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="M39" s="23" t="s">
+        <v>174</v>
+      </c>
+      <c r="N39" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O39" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="P39" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q39" s="20"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="17"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F40" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>186</v>
+      </c>
+      <c r="H40" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="I40" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J40" s="19">
+        <v>30</v>
+      </c>
+      <c r="K40" s="20" t="s">
+        <v>188</v>
+      </c>
+      <c r="L40" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="M40" s="23" t="s">
+        <v>189</v>
+      </c>
+      <c r="N40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O40" s="21" t="s">
+        <v>190</v>
+      </c>
+      <c r="P40" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q40" s="20"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="17"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J41" s="19">
+        <v>36</v>
+      </c>
+      <c r="K41" s="20" t="s">
+        <v>192</v>
+      </c>
+      <c r="L41" s="23" t="s">
+        <v>193</v>
+      </c>
+      <c r="M41" s="23" t="s">
+        <v>194</v>
+      </c>
+      <c r="N41" s="23" t="s">
+        <v>195</v>
+      </c>
+      <c r="O41" s="21" t="s">
+        <v>196</v>
+      </c>
+      <c r="P41" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q41" s="20"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="17"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G42" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H42" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I42" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="J42" s="19">
+        <v>100</v>
+      </c>
+      <c r="K42" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="L42" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M42" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O42" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="P42" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q42" s="20"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="17"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="J43" s="19">
+        <v>36</v>
+      </c>
+      <c r="K43" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="L43" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M43" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N43" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O43" s="21" t="s">
+        <v>206</v>
+      </c>
+      <c r="P43" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q43" s="20"/>
+      <c r="R43" s="18"/>
+      <c r="S43" s="18"/>
+      <c r="T43" s="17"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G44" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H44" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I44" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="J44" s="19">
+        <v>82</v>
+      </c>
+      <c r="K44" s="20" t="s">
+        <v>207</v>
+      </c>
+      <c r="L44" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M44" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N44" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O44" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="P44" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q44" s="20"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="17"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I45" s="7" t="s">
+        <v>84</v>
+      </c>
+      <c r="J45" s="19">
+        <v>82</v>
+      </c>
+      <c r="K45" s="20" t="s">
+        <v>209</v>
+      </c>
+      <c r="L45" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M45" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N45" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O45" s="21" t="s">
+        <v>210</v>
+      </c>
+      <c r="P45" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q45" s="20"/>
+      <c r="R45" s="18"/>
+      <c r="S45" s="18"/>
+      <c r="T45" s="17"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>198</v>
+      </c>
+      <c r="G46" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="H46" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I46" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="J46" s="19">
+        <v>82</v>
+      </c>
+      <c r="K46" s="20" t="s">
+        <v>211</v>
+      </c>
+      <c r="L46" s="23" t="s">
+        <v>201</v>
+      </c>
+      <c r="M46" s="23" t="s">
+        <v>202</v>
+      </c>
+      <c r="N46" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O46" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="P46" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q46" s="20"/>
+      <c r="R46" s="18"/>
+      <c r="S46" s="18"/>
+      <c r="T46" s="17"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="I47" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J47" s="19">
+        <v>1</v>
+      </c>
+      <c r="K47" s="20" t="s">
+        <v>216</v>
+      </c>
+      <c r="L47" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M47" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N47" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O47" s="21" t="s">
+        <v>218</v>
+      </c>
+      <c r="P47" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q47" s="20"/>
+      <c r="R47" s="18"/>
+      <c r="S47" s="18"/>
+      <c r="T47" s="17"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="G48" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="H48" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I48" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J48" s="19">
+        <v>82</v>
+      </c>
+      <c r="K48" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="L48" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M48" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N48" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O48" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="P48" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q48" s="20"/>
+      <c r="R48" s="18"/>
+      <c r="S48" s="18"/>
+      <c r="T48" s="17"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E49" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H49" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J49" s="19">
+        <v>29</v>
+      </c>
+      <c r="K49" s="20" t="s">
+        <v>221</v>
+      </c>
+      <c r="L49" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M49" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N49" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O49" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="P49" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="18"/>
+      <c r="S49" s="18"/>
+      <c r="T49" s="17"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E50" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G50" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H50" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="I50" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J50" s="19">
+        <v>59</v>
+      </c>
+      <c r="K50" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="L50" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M50" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N50" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O50" s="21" t="s">
+        <v>224</v>
+      </c>
+      <c r="P50" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q50" s="20"/>
+      <c r="R50" s="18"/>
+      <c r="S50" s="18"/>
+      <c r="T50" s="17"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E51" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>213</v>
+      </c>
+      <c r="G51" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="H51" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="I51" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J51" s="19">
+        <v>43</v>
+      </c>
+      <c r="K51" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="L51" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="M51" s="23" t="s">
+        <v>217</v>
+      </c>
+      <c r="N51" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O51" s="21" t="s">
+        <v>226</v>
+      </c>
+      <c r="P51" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q51" s="20"/>
+      <c r="R51" s="18"/>
+      <c r="S51" s="18"/>
+      <c r="T51" s="17"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="G52" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="H52" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I52" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="J52" s="19">
+        <v>36</v>
+      </c>
+      <c r="K52" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="L52" s="23" t="s">
+        <v>231</v>
+      </c>
+      <c r="M52" s="23" t="s">
+        <v>232</v>
+      </c>
+      <c r="N52" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O52" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="P52" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q52" s="20"/>
+      <c r="R52" s="18"/>
+      <c r="S52" s="18"/>
+      <c r="T52" s="17"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J53" s="19">
+        <v>100</v>
+      </c>
+      <c r="K53" s="20" t="s">
+        <v>236</v>
+      </c>
+      <c r="L53" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M53" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N53" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>239</v>
+      </c>
+      <c r="P53" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q53" s="20"/>
+      <c r="R53" s="18"/>
+      <c r="S53" s="18"/>
+      <c r="T53" s="17"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G54" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H54" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I54" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J54" s="19">
+        <v>36</v>
+      </c>
+      <c r="K54" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="L54" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M54" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O54" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="P54" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q54" s="20"/>
+      <c r="R54" s="18"/>
+      <c r="S54" s="18"/>
+      <c r="T54" s="17"/>
+    </row>
+    <row r="55">
+      <c r="A55" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="I55" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J55" s="19">
+        <v>29</v>
+      </c>
+      <c r="K55" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="L55" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M55" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N55" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O55" s="21" t="s">
+        <v>243</v>
+      </c>
+      <c r="P55" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q55" s="20"/>
+      <c r="R55" s="18"/>
+      <c r="S55" s="18"/>
+      <c r="T55" s="17"/>
+    </row>
+    <row r="56">
+      <c r="A56" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D56" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F56" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H56" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="I56" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J56" s="19">
+        <v>59</v>
+      </c>
+      <c r="K56" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="L56" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M56" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N56" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O56" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="P56" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q56" s="20"/>
+      <c r="R56" s="18"/>
+      <c r="S56" s="18"/>
+      <c r="T56" s="17"/>
+    </row>
+    <row r="57">
+      <c r="A57" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="I57" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J57" s="19">
+        <v>43</v>
+      </c>
+      <c r="K57" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="L57" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M57" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N57" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O57" s="21" t="s">
+        <v>247</v>
+      </c>
+      <c r="P57" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q57" s="20"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="17"/>
+    </row>
+    <row r="58">
+      <c r="A58" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F58" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G58" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H58" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="I58" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J58" s="19">
+        <v>82</v>
+      </c>
+      <c r="K58" s="20" t="s">
+        <v>248</v>
+      </c>
+      <c r="L58" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M58" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N58" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O58" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="P58" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q58" s="20"/>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="17"/>
+    </row>
+    <row r="59">
+      <c r="A59" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="F59" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="I59" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J59" s="19">
+        <v>28</v>
+      </c>
+      <c r="K59" s="20" t="s">
+        <v>250</v>
+      </c>
+      <c r="L59" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="M59" s="23" t="s">
+        <v>238</v>
+      </c>
+      <c r="N59" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O59" s="21" t="s">
+        <v>251</v>
+      </c>
+      <c r="P59" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="Q59" s="20" t="s">
+        <v>253</v>
+      </c>
+      <c r="R59" s="18" t="s">
+        <v>254</v>
+      </c>
+      <c r="S59" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="T59" s="17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C60" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D60" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E60" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F60" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="G60" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="H60" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="I60" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="J60" s="19">
+        <v>36</v>
+      </c>
+      <c r="K60" s="20" t="s">
+        <v>258</v>
+      </c>
+      <c r="L60" s="23" t="s">
+        <v>259</v>
+      </c>
+      <c r="M60" s="23" t="s">
+        <v>260</v>
+      </c>
+      <c r="N60" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O60" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="P60" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q60" s="20"/>
+      <c r="R60" s="18"/>
+      <c r="S60" s="18"/>
+      <c r="T60" s="17"/>
+    </row>
+    <row r="61">
+      <c r="A61" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C61" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E61" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F61" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="G61" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="H61" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I61" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="J61" s="19">
+        <v>0</v>
+      </c>
+      <c r="K61" s="20" t="s">
+        <v>263</v>
+      </c>
+      <c r="L61" s="23" t="s">
+        <v>264</v>
+      </c>
+      <c r="M61" s="23" t="s">
+        <v>265</v>
+      </c>
+      <c r="N61" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O61" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="P61" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q61" s="20"/>
+      <c r="R61" s="18"/>
+      <c r="S61" s="18"/>
+      <c r="T61" s="17"/>
+    </row>
+    <row r="62">
+      <c r="A62" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B22" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="C22" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="18" t="s">
+      <c r="B62" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="C62" s="18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="E22" s="18" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>160</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="H22" s="22" t="s">
+      <c r="E62" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="F62" s="18" t="s">
+        <v>267</v>
+      </c>
+      <c r="G62" s="22" t="s">
+        <v>268</v>
+      </c>
+      <c r="H62" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="I22" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="J22" s="19">
-        <v>100</v>
-      </c>
-      <c r="K22" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="L22" s="23" t="s">
-        <v>163</v>
-      </c>
-      <c r="M22" s="23" t="s">
-        <v>164</v>
-      </c>
-      <c r="N22" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="O22" s="21" t="s">
-        <v>165</v>
-      </c>
-      <c r="P22" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="Q22" s="20" t="s">
-        <v>167</v>
-      </c>
-      <c r="R22" s="18" t="s">
+      <c r="I62" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="J62" s="19">
+        <v>36</v>
+      </c>
+      <c r="K62" s="20" t="s">
+        <v>269</v>
+      </c>
+      <c r="L62" s="23" t="s">
+        <v>270</v>
+      </c>
+      <c r="M62" s="23" t="s">
+        <v>271</v>
+      </c>
+      <c r="N62" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="O62" s="21" t="s">
+        <v>272</v>
+      </c>
+      <c r="P62" s="12" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q62" s="20" t="s">
+        <v>274</v>
+      </c>
+      <c r="R62" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="S22" s="18" t="s">
+      <c r="S62" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="T22" s="17" t="s">
+      <c r="T62" s="17" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>